<commit_message>
added Practice problems and updated lecture
</commit_message>
<xml_diff>
--- a/Excel/Excel Assignment Concatenate, Date formulas.xlsx
+++ b/Excel/Excel Assignment Concatenate, Date formulas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishan\Desktop\Bootcamp.Info\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287DCECE-CCDD-4754-819A-D22A42426858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CF097A-6F19-44E4-B7CB-A5687230FF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1CACAED8-3174-4CCE-811F-5ADACE73B21C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CACAED8-3174-4CCE-811F-5ADACE73B21C}"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="1" r:id="rId1"/>
@@ -494,13 +494,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993AB60E-D262-4E4E-A3FE-7EECEAB003E6}">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,14 +858,14 @@
         <v>113</v>
       </c>
       <c r="I1"/>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -895,12 +895,12 @@
         <f>C2&amp; ","&amp;G2&amp;"("&amp;F2&amp;")"</f>
         <v>Montgomery , Alabama (AL )</v>
       </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -930,12 +930,12 @@
         <f t="shared" ref="H3:H49" si="1">C3&amp; ","&amp;G3&amp;"("&amp;F3&amp;")"</f>
         <v>Juneau , Alaska (AK )</v>
       </c>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -965,12 +965,12 @@
         <f t="shared" si="1"/>
         <v>Phoenix , Arizona (AZ )</v>
       </c>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1000,12 +1000,12 @@
         <f t="shared" si="1"/>
         <v>Little Rock , Arkansas (AR )</v>
       </c>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1035,12 +1035,12 @@
         <f t="shared" si="1"/>
         <v>Sacramento , California (CA )</v>
       </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1070,12 +1070,12 @@
         <f t="shared" si="1"/>
         <v>Denver , Colorado (CO )</v>
       </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -1105,12 +1105,12 @@
         <f t="shared" si="1"/>
         <v>Hartford , Connecticut (CT )</v>
       </c>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2313,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F9A2A9-87B7-4DB5-A01C-89C6B277FF41}">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2354,30 +2354,30 @@
       <c r="K1" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <f ca="1">TODAY()</f>
-        <v>44504</v>
-      </c>
-      <c r="C2" s="10">
+        <v>44506</v>
+      </c>
+      <c r="C2" s="8">
         <v>44514</v>
       </c>
       <c r="D2">
         <f ca="1">C2-B2</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <f>WEEKDAY(C2)</f>
@@ -2397,28 +2397,28 @@
       <c r="L2" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <f t="shared" ref="B3:B5" ca="1" si="0">TODAY()</f>
-        <v>44504</v>
-      </c>
-      <c r="C3" s="10">
+        <v>44506</v>
+      </c>
+      <c r="C3" s="8">
         <v>44582</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" ca="1" si="1">C3-B3</f>
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="2">WEEKDAY(C3)</f>
@@ -2438,28 +2438,28 @@
       <c r="L3" t="s">
         <v>119</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44504</v>
-      </c>
-      <c r="C4" s="10">
+        <v>44506</v>
+      </c>
+      <c r="C4" s="8">
         <v>44647</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
@@ -2479,28 +2479,28 @@
       <c r="L4" t="s">
         <v>120</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>44504</v>
-      </c>
-      <c r="C5" s="10">
+        <v>44506</v>
+      </c>
+      <c r="C5" s="8">
         <v>44555</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
@@ -2520,13 +2520,13 @@
       <c r="L5" t="s">
         <v>121</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="K6">
@@ -2535,13 +2535,13 @@
       <c r="L6" t="s">
         <v>122</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="K7">
@@ -2550,13 +2550,13 @@
       <c r="L7" t="s">
         <v>123</v>
       </c>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="K8">
@@ -2565,13 +2565,13 @@
       <c r="L8" t="s">
         <v>124</v>
       </c>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>